<commit_message>
Integration with supabase (no more localhost to test, you can still use the XXX_unused to test using localhost)
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\price-calculator\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c3ef52a6b12a640/Dokumen/GitHub/React Store Application/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1B1DEA-5C21-467A-857D-842B518649A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{32893FA9-AE84-5041-89A8-DBB0FCBB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B90C3F82-A8B4-4523-A2DA-48B49FB21D65}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$33</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -42,53 +45,234 @@
     <t>image</t>
   </si>
   <si>
-    <t>Sticker 1</t>
-  </si>
-  <si>
     <t>Sticker</t>
   </si>
   <si>
-    <t>Keychain 1</t>
-  </si>
-  <si>
     <t>Keychain</t>
   </si>
   <si>
-    <t>Poster 1</t>
-  </si>
-  <si>
-    <t>Poster</t>
-  </si>
-  <si>
-    <t>Sticker 2</t>
-  </si>
-  <si>
-    <t>Keychain 2</t>
-  </si>
-  <si>
-    <t>Poster 2</t>
-  </si>
-  <si>
     <t>qty</t>
   </si>
   <si>
-    <t>image1.jpg</t>
-  </si>
-  <si>
-    <t>image2.jpg</t>
-  </si>
-  <si>
-    <t>image3.jpg</t>
+    <t>HAPPY joy</t>
+  </si>
+  <si>
+    <t>HATING churros</t>
+  </si>
+  <si>
+    <t>KILLER churros</t>
+  </si>
+  <si>
+    <t>HOLO nori</t>
+  </si>
+  <si>
+    <t>HOLO custard</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>No way</t>
+  </si>
+  <si>
+    <t>Starry nori</t>
+  </si>
+  <si>
+    <t>Zooming churros</t>
+  </si>
+  <si>
+    <t>Sleepy joy</t>
+  </si>
+  <si>
+    <t>Holo joy</t>
+  </si>
+  <si>
+    <t>Bike churros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merry go round </t>
+  </si>
+  <si>
+    <t>Safe place custard</t>
+  </si>
+  <si>
+    <t>Unicycle joy</t>
+  </si>
+  <si>
+    <t>Prot prot</t>
+  </si>
+  <si>
+    <t>I don’t care joy</t>
+  </si>
+  <si>
+    <t>Worried churros</t>
+  </si>
+  <si>
+    <t>Starry Custard</t>
+  </si>
+  <si>
+    <t>It's okay</t>
+  </si>
+  <si>
+    <t>Giant churros</t>
+  </si>
+  <si>
+    <t>Churros day care</t>
+  </si>
+  <si>
+    <t>Fool nori</t>
+  </si>
+  <si>
+    <t>Basic math joy</t>
+  </si>
+  <si>
+    <t>Better together</t>
+  </si>
+  <si>
+    <t>Any a5 prints</t>
+  </si>
+  <si>
+    <t>Choo choo/Joy a5</t>
+  </si>
+  <si>
+    <t>Lanyard</t>
+  </si>
+  <si>
+    <t>Taiyaki girl</t>
+  </si>
+  <si>
+    <t>Playdate a4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pouch </t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Prints</t>
+  </si>
+  <si>
+    <t>Artboard 1.png</t>
+  </si>
+  <si>
+    <t>Artboard 3.png</t>
+  </si>
+  <si>
+    <t>Artboard 4.png</t>
+  </si>
+  <si>
+    <t>Artboard 5.png</t>
+  </si>
+  <si>
+    <t>Artboard 6.png</t>
+  </si>
+  <si>
+    <t>Artboard 7.png</t>
+  </si>
+  <si>
+    <t>Studying churros</t>
+  </si>
+  <si>
+    <t>Artboard 8.png</t>
+  </si>
+  <si>
+    <t>Artboard 9.png</t>
+  </si>
+  <si>
+    <t>Artboard 10.png</t>
+  </si>
+  <si>
+    <t>Artboard 11.png</t>
+  </si>
+  <si>
+    <t>Artboard 12.png</t>
+  </si>
+  <si>
+    <t>Artboard 13.png</t>
+  </si>
+  <si>
+    <t>Artboard 14.png</t>
+  </si>
+  <si>
+    <t>Artboard 15.png</t>
+  </si>
+  <si>
+    <t>Artboard 17.png</t>
+  </si>
+  <si>
+    <t>Artboard 18.png</t>
+  </si>
+  <si>
+    <t>Artboard 19.png</t>
+  </si>
+  <si>
+    <t>Artboard 20.png</t>
+  </si>
+  <si>
+    <t>Artboard 21.png</t>
+  </si>
+  <si>
+    <t>Artboard 22.png</t>
+  </si>
+  <si>
+    <t>Artboard 24.png</t>
+  </si>
+  <si>
+    <t>Artboard 25.png</t>
+  </si>
+  <si>
+    <t>Artboard 26.png</t>
+  </si>
+  <si>
+    <t>Artboard 23.png</t>
+  </si>
+  <si>
+    <t>Artboard 27.png</t>
+  </si>
+  <si>
+    <t>Artboard 28.png</t>
+  </si>
+  <si>
+    <t>Artboard 31.png</t>
+  </si>
+  <si>
+    <t>Artboard 30.png</t>
+  </si>
+  <si>
+    <t>Artboard 32.png</t>
+  </si>
+  <si>
+    <t>Artboard 33.png</t>
+  </si>
+  <si>
+    <t>Artboard 34.png</t>
+  </si>
+  <si>
+    <t>Artboard 16.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,8 +298,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,13 +581,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="116" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -421,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -429,16 +619,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>5.99</v>
+        <v>11000</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -449,16 +639,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>7.99</v>
+        <v>11000</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -469,16 +659,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>15.99</v>
+        <v>11000</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -492,13 +682,13 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>4.99</v>
+        <v>11000</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -512,13 +702,13 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>6.99</v>
+        <v>11000</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -532,19 +722,541 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>12.99</v>
+        <v>9000</v>
       </c>
       <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>9000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>8000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>11000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="F7">
+      <c r="C11">
+        <v>11000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>9000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>9000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>9000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>9000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>9000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>8000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>9000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>9000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>45000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>50000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>50000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>11000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>18000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>25000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>55000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>35000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>65000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>50000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>30000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33">
+        <v>9000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct the filtering for product list and Transaction list
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c3ef52a6b12a640/Dokumen/GitHub/React Store Application/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{32893FA9-AE84-5041-89A8-DBB0FCBB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B90C3F82-A8B4-4523-A2DA-48B49FB21D65}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{32893FA9-AE84-5041-89A8-DBB0FCBB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6BD3489-96D2-4648-8614-FC4C966F9684}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,6 +316,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,19 +620,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>11000</v>
+        <v>35000</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -636,10 +640,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>11000</v>
@@ -648,7 +652,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -656,19 +660,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -676,19 +680,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>11000</v>
+        <v>9000</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -696,19 +700,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>11000</v>
+        <v>9000</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -716,19 +720,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>9000</v>
+        <v>25000</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -736,19 +740,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>9000</v>
+        <v>50000</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -756,19 +760,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>8000</v>
+        <v>50000</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -776,19 +780,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C10">
-        <v>11000</v>
+        <v>45000</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -796,10 +800,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>11000</v>
@@ -808,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -816,19 +820,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -836,19 +840,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
       <c r="C13">
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -856,10 +860,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>9000</v>
@@ -868,7 +872,7 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -876,19 +880,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -896,19 +900,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>9000</v>
+        <v>24</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8000</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -916,19 +920,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1">
         <v>8000</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -936,19 +940,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8000</v>
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>11000</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -956,19 +960,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C19">
-        <v>9000</v>
+        <v>55000</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -976,10 +980,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>9000</v>
@@ -988,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -996,19 +1000,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1">
-        <v>8000</v>
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>9000</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1016,19 +1020,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1036,19 +1040,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C23">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1056,19 +1060,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
       <c r="C24">
-        <v>50000</v>
+        <v>8000</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1076,19 +1080,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>11000</v>
+        <v>9000</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1096,19 +1100,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>18000</v>
+        <v>11000</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1116,19 +1120,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
       <c r="C27">
-        <v>25000</v>
+        <v>9000</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1136,19 +1140,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1156,19 +1160,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C29">
-        <v>35000</v>
+        <v>9000</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1196,19 +1200,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>50000</v>
+        <v>9000</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1216,19 +1220,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C32">
-        <v>30000</v>
+        <v>9000</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1236,26 +1240,30 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F33" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
+      <sortCondition ref="B1:B33"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update item list and remove image in cart view
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c3ef52a6b12a640/Dokumen/GitHub/React Store Application/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{32893FA9-AE84-5041-89A8-DBB0FCBB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6BD3489-96D2-4648-8614-FC4C966F9684}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{32893FA9-AE84-5041-89A8-DBB0FCBB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C71CB8E-648F-4843-AE59-578460488417}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>Artboard 16.png</t>
+  </si>
+  <si>
+    <t>Photobook</t>
+  </si>
+  <si>
+    <t>Star Keychain</t>
+  </si>
+  <si>
+    <t>Artboard 35.png</t>
+  </si>
+  <si>
+    <t>Mini poster</t>
+  </si>
+  <si>
+    <t>Artboard 36.png</t>
   </si>
 </sst>
 </file>
@@ -319,6 +334,10 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -585,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,19 +1019,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="C21">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1020,19 +1039,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C22">
-        <v>50000</v>
+        <v>9000</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1040,19 +1059,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C23">
-        <v>30000</v>
+        <v>120000</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1060,19 +1079,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C24">
-        <v>8000</v>
+        <v>50000</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1080,19 +1099,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C25">
-        <v>9000</v>
+        <v>30000</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1100,19 +1119,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>11000</v>
+        <v>8000</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1120,10 +1139,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>9000</v>
@@ -1132,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1140,19 +1159,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1160,19 +1179,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C29">
-        <v>9000</v>
+        <v>75000</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1180,19 +1199,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C30">
-        <v>65000</v>
+        <v>9000</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1200,19 +1219,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
         <v>15</v>
       </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
       <c r="C31">
-        <v>9000</v>
+        <v>8000</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1220,10 +1239,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>9000</v>
@@ -1232,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1240,27 +1259,87 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>65000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>9000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>9000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="C33">
+      <c r="C36">
         <v>11000</v>
       </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
         <v>50</v>
       </c>
-      <c r="F33">
+      <c r="F36">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F33" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
       <sortCondition ref="B1:B33"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
fixed wrong item list
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c3ef52a6b12a640/Dokumen/GitHub/React Store Application/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E019E667-97D1-43F2-86F1-5A2ED696F857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25013E8C-F748-4707-8556-9CBC38D719CF}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{E019E667-97D1-43F2-86F1-5A2ED696F857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C77E7D48-6C66-4252-AE66-FA1938F6C508}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t xml:space="preserve">enamel bundle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other </t>
   </si>
   <si>
     <t>hang in there enamel</t>
@@ -368,6 +365,10 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -636,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,19 +670,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>12000</v>
+        <v>35000</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -689,10 +690,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>12000</v>
@@ -701,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -709,19 +710,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>12000</v>
+        <v>18000</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -729,19 +730,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -749,19 +750,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>12000</v>
+        <v>35000</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -769,19 +770,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C7">
-        <v>9000</v>
+        <v>50000</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -789,19 +790,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C8">
-        <v>8000</v>
+        <v>25000</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -809,19 +810,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C9">
-        <v>12000</v>
+        <v>230000</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -829,19 +830,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C10">
-        <v>12000</v>
+        <v>50000</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -849,19 +850,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>9000</v>
+        <v>45000</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -869,19 +870,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C12">
-        <v>9000</v>
+        <v>120000</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -889,19 +890,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -909,19 +910,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -929,19 +930,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -949,19 +950,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -969,19 +970,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="1">
-        <v>8000</v>
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>12000</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -989,19 +990,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C18">
-        <v>9000</v>
+        <v>190000</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1009,19 +1010,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>9000</v>
+        <v>79</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8000</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1049,19 +1050,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C21">
-        <v>45000</v>
+        <v>55000</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1069,19 +1070,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>50000</v>
+        <v>12000</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1089,19 +1090,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>50000</v>
+        <v>9000</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1109,19 +1110,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1129,19 +1130,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C25">
-        <v>18000</v>
+        <v>120000</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1149,19 +1150,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>35000</v>
+        <v>50000</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1169,19 +1170,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>35000</v>
+        <v>8000</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1189,19 +1190,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C28">
-        <v>50000</v>
+        <v>200000</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1209,19 +1210,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C29">
-        <v>9000</v>
+        <v>150000</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1229,19 +1230,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C30">
-        <v>120000</v>
+        <v>180000</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1249,19 +1250,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>55000</v>
+        <v>9000</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1269,19 +1270,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>25000</v>
+        <v>12000</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1289,19 +1290,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>230000</v>
+        <v>9000</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1309,19 +1310,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C34">
-        <v>120000</v>
+        <v>8000</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1329,19 +1330,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="C35">
-        <v>55000</v>
+        <v>9000</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1349,19 +1350,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C36">
-        <v>190000</v>
+        <v>50000</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1369,19 +1370,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>200000</v>
+        <v>9000</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1389,19 +1390,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C38">
-        <v>180000</v>
+        <v>120000</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1409,19 +1410,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>150000</v>
+        <v>9000</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1429,19 +1430,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C40">
-        <v>120000</v>
+        <v>12000</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1449,19 +1450,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C41">
-        <v>50000</v>
+        <v>55000</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1470,7 +1471,7 @@
   </sheetData>
   <autoFilter ref="A1:F41" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F41">
-      <sortCondition ref="A1:A41"/>
+      <sortCondition ref="B1:B41"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>